<commit_message>
Completed Modal, modified Controller func
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>route_id</t>
   </si>
@@ -124,7 +124,40 @@
     <t>ALUVA</t>
   </si>
   <si>
-    <t>City_id</t>
+    <t>0009</t>
+  </si>
+  <si>
+    <t>0012</t>
+  </si>
+  <si>
+    <t>0015</t>
+  </si>
+  <si>
+    <t>0016</t>
+  </si>
+  <si>
+    <t>0018</t>
+  </si>
+  <si>
+    <t>0019</t>
+  </si>
+  <si>
+    <t>0020</t>
+  </si>
+  <si>
+    <t>0021</t>
+  </si>
+  <si>
+    <t>0022</t>
+  </si>
+  <si>
+    <t>0023</t>
+  </si>
+  <si>
+    <t>0024</t>
+  </si>
+  <si>
+    <t>0025</t>
   </si>
 </sst>
 </file>
@@ -468,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +529,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -504,7 +537,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -512,7 +545,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -520,7 +553,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -528,7 +561,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -536,152 +569,144 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
+      <c r="A8" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
+      <c r="A9" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
+      <c r="A10" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>20</v>
+      <c r="A11" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
+      <c r="A12" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3</v>
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1</v>
+      <c r="A14" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>2</v>
+      <c r="A15" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>3</v>
+      <c r="A16" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>4</v>
+      <c r="A17" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>5</v>
+      <c r="A18" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>6</v>
+      <c r="A19" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>7</v>
+      <c r="A20" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>8</v>
+      <c r="A21" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>9</v>
+      <c r="A22" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>10</v>
+      <c r="A23" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>11</v>
+      <c r="A24" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>12</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="1"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>